<commit_message>
completed end-to-end test pulling data from test case and using common methods
</commit_message>
<xml_diff>
--- a/src/tests/demoUI/data/demoOrangeHrmTestData.xlsx
+++ b/src/tests/demoUI/data/demoOrangeHrmTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mthomas\Documents\mtf-automation-testing-ui\src\tests\shared\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mthomas\Documents\mtf-automation-testing-ui\src\tests\demoUI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E606E736-F6DB-411B-B612-C567636C5C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F9267E-6EF8-4117-8525-660D67F82ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3FAEF57A-74CB-4873-83C5-7175CED35448}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>SU-TC001</t>
   </si>
@@ -51,61 +51,43 @@
     <t>TEST_CASE</t>
   </si>
   <si>
-    <t>USER_NAME</t>
-  </si>
-  <si>
-    <t>UserTestNameA</t>
-  </si>
-  <si>
-    <t>UserTestNameB</t>
-  </si>
-  <si>
     <t>C-TC001</t>
   </si>
   <si>
-    <t>C-TC002</t>
-  </si>
-  <si>
-    <t>USER_ROLE</t>
-  </si>
-  <si>
-    <t>EMPLOYEE_NAME</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
-  </si>
-  <si>
-    <t>CONFIRM_PASSWORD</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
-    <t>ESS</t>
-  </si>
-  <si>
-    <t>Joe Clark</t>
-  </si>
-  <si>
-    <t>Jane Clark</t>
-  </si>
-  <si>
     <t>Enabled</t>
   </si>
   <si>
-    <t>Disabled</t>
-  </si>
-  <si>
-    <t>joeclark123</t>
-  </si>
-  <si>
-    <t>janeclark123</t>
-  </si>
-  <si>
     <t>File</t>
+  </si>
+  <si>
+    <t>Timothy Lewis Amiano</t>
+  </si>
+  <si>
+    <t>password1</t>
+  </si>
+  <si>
+    <t>timothy.amiano</t>
+  </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>User Role</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -473,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E585723F-DA52-4C5A-A7AB-E6B3EDE8D02A}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -484,7 +466,7 @@
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.77734375" customWidth="1"/>
     <col min="3" max="3" width="18.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.77734375" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
@@ -495,68 +477,45 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -580,7 +539,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
completed add the delete step
</commit_message>
<xml_diff>
--- a/src/tests/demoUI/data/demoOrangeHrmTestData.xlsx
+++ b/src/tests/demoUI/data/demoOrangeHrmTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mthomas\Documents\mtf-automation-testing-ui\src\tests\demoUI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4A5FAE-39CA-400D-AA44-139BFE994343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2AE652-5B82-4A0A-BC95-06FCA509D62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25960" yWindow="2440" windowWidth="25690" windowHeight="11770" xr2:uid="{3FAEF57A-74CB-4873-83C5-7175CED35448}"/>
+    <workbookView xWindow="744" yWindow="732" windowWidth="21000" windowHeight="11772" xr2:uid="{3FAEF57A-74CB-4873-83C5-7175CED35448}"/>
   </bookViews>
   <sheets>
     <sheet name="Add-User" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>